<commit_message>
SAving and loading for player/weapons done
</commit_message>
<xml_diff>
--- a/OpenGLEngine/OpenGLEngine/SaveData/_SaveFormatDescriptions.xlsx
+++ b/OpenGLEngine/OpenGLEngine/SaveData/_SaveFormatDescriptions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>GameObjects</t>
   </si>
@@ -82,9 +82,6 @@
     <t>currentHealth</t>
   </si>
   <si>
-    <t>maxHealth</t>
-  </si>
-  <si>
     <t>Quests</t>
   </si>
   <si>
@@ -149,6 +146,33 @@
   </si>
   <si>
     <t>isComplete</t>
+  </si>
+  <si>
+    <t>Yaw</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>WEAPON_Data</t>
+  </si>
+  <si>
+    <t>currentWeaponID</t>
+  </si>
+  <si>
+    <t>weaponID</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>range</t>
   </si>
 </sst>
 </file>
@@ -490,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,112 +645,134 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>42</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>43</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" t="s">
         <v>34</v>
-      </c>
-      <c r="F15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>39</v>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>